<commit_message>
Updates on AI weight
</commit_message>
<xml_diff>
--- a/产出平衡.xlsx
+++ b/产出平衡.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\GitHub\Sistine_civ6mod\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{142F9D45-F25A-465C-BAD2-156A6360E1BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E495D417-26AA-4AE3-A759-1EB9935AF083}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{E8AAC43B-5A54-406D-B95D-5DF386335546}"/>
+    <workbookView xWindow="3264" yWindow="444" windowWidth="19500" windowHeight="11688" xr2:uid="{E8AAC43B-5A54-406D-B95D-5DF386335546}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -465,8 +465,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0B8A3E97-52CE-4D75-8992-93CFC5B46B46}">
   <dimension ref="A1:O23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F20" sqref="F20"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="G22" sqref="G22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -1001,7 +1001,7 @@
         <v>1</v>
       </c>
       <c r="D18">
-        <v>1.25</v>
+        <v>1.3</v>
       </c>
       <c r="E18">
         <v>1.1000000000000001</v>
@@ -1014,7 +1014,7 @@
       </c>
       <c r="H18">
         <f>SUM(B18:G18)</f>
-        <v>6.55</v>
+        <v>6.6000000000000005</v>
       </c>
       <c r="J18">
         <f>B18-1</f>
@@ -1026,7 +1026,7 @@
       </c>
       <c r="L18">
         <f t="shared" si="12"/>
-        <v>0.25</v>
+        <v>0.30000000000000004</v>
       </c>
       <c r="M18">
         <f t="shared" si="12"/>
@@ -1052,7 +1052,7 @@
         <v>1.1000000000000001</v>
       </c>
       <c r="D19">
-        <v>1.45</v>
+        <v>1.4</v>
       </c>
       <c r="E19">
         <v>1.1000000000000001</v>
@@ -1065,7 +1065,7 @@
       </c>
       <c r="H19">
         <f t="shared" ref="H19:H23" si="13">SUM(B19:G19)</f>
-        <v>7.25</v>
+        <v>7.1999999999999993</v>
       </c>
       <c r="J19">
         <f>B19-B18</f>
@@ -1077,7 +1077,7 @@
       </c>
       <c r="L19">
         <f t="shared" si="14"/>
-        <v>0.19999999999999996</v>
+        <v>9.9999999999999867E-2</v>
       </c>
       <c r="M19">
         <f t="shared" si="14"/>
@@ -1097,13 +1097,13 @@
         <v>8</v>
       </c>
       <c r="B20">
-        <v>1.65</v>
+        <v>1.35</v>
       </c>
       <c r="C20">
-        <v>1.3</v>
+        <v>1.45</v>
       </c>
       <c r="D20">
-        <v>1.55</v>
+        <v>1.5</v>
       </c>
       <c r="E20">
         <v>1.25</v>
@@ -1116,15 +1116,15 @@
       </c>
       <c r="H20">
         <f t="shared" si="13"/>
-        <v>7.5</v>
+        <v>7.3</v>
       </c>
       <c r="J20">
         <f t="shared" ref="J20:J23" si="15">B20-B19</f>
-        <v>0.19999999999999996</v>
+        <v>-9.9999999999999867E-2</v>
       </c>
       <c r="K20">
         <f t="shared" si="14"/>
-        <v>0.19999999999999996</v>
+        <v>0.34999999999999987</v>
       </c>
       <c r="L20">
         <f t="shared" si="14"/>
@@ -1148,10 +1148,10 @@
         <v>9</v>
       </c>
       <c r="B21">
-        <v>1.75</v>
+        <v>1.5</v>
       </c>
       <c r="C21">
-        <v>1.4</v>
+        <v>1.6</v>
       </c>
       <c r="D21">
         <v>1.55</v>
@@ -1167,19 +1167,19 @@
       </c>
       <c r="H21">
         <f t="shared" si="13"/>
-        <v>7.4999999999999991</v>
+        <v>7.45</v>
       </c>
       <c r="J21">
         <f t="shared" si="15"/>
-        <v>0.10000000000000009</v>
+        <v>0.14999999999999991</v>
       </c>
       <c r="K21">
         <f t="shared" si="14"/>
-        <v>9.9999999999999867E-2</v>
+        <v>0.15000000000000013</v>
       </c>
       <c r="L21">
         <f t="shared" si="14"/>
-        <v>0</v>
+        <v>5.0000000000000044E-2</v>
       </c>
       <c r="M21">
         <f t="shared" si="14"/>
@@ -1199,7 +1199,7 @@
         <v>10</v>
       </c>
       <c r="B22">
-        <v>1.75</v>
+        <v>1.5</v>
       </c>
       <c r="C22">
         <v>1.7</v>
@@ -1208,7 +1208,7 @@
         <v>1.55</v>
       </c>
       <c r="E22">
-        <v>1.5</v>
+        <v>1.4</v>
       </c>
       <c r="F22">
         <v>1</v>
@@ -1218,7 +1218,7 @@
       </c>
       <c r="H22">
         <f t="shared" si="13"/>
-        <v>7.8</v>
+        <v>7.45</v>
       </c>
       <c r="J22">
         <f t="shared" si="15"/>
@@ -1226,7 +1226,7 @@
       </c>
       <c r="K22">
         <f t="shared" si="14"/>
-        <v>0.30000000000000004</v>
+        <v>9.9999999999999867E-2</v>
       </c>
       <c r="L22">
         <f t="shared" si="14"/>
@@ -1234,7 +1234,7 @@
       </c>
       <c r="M22">
         <f t="shared" si="14"/>
-        <v>0.10000000000000009</v>
+        <v>0</v>
       </c>
       <c r="N22">
         <f t="shared" si="14"/>
@@ -1250,7 +1250,7 @@
         <v>11</v>
       </c>
       <c r="B23">
-        <v>1.75</v>
+        <v>1.5</v>
       </c>
       <c r="C23">
         <v>1.8</v>
@@ -1259,7 +1259,7 @@
         <v>1.55</v>
       </c>
       <c r="E23">
-        <v>1.5</v>
+        <v>1.4</v>
       </c>
       <c r="F23">
         <v>1</v>
@@ -1269,7 +1269,7 @@
       </c>
       <c r="H23">
         <f t="shared" si="13"/>
-        <v>7.8999999999999995</v>
+        <v>7.55</v>
       </c>
       <c r="J23">
         <f t="shared" si="15"/>

</xml_diff>